<commit_message>
Rework parser for raw text input
</commit_message>
<xml_diff>
--- a/input/L3.xlsx
+++ b/input/L3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>interface type</t>
   </si>
@@ -40,24 +40,51 @@
     <t>gigabitethernet</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
     <t>10.32.5.5</t>
   </si>
   <si>
     <t>255.255.240.0</t>
   </si>
   <si>
+    <t>ESGI-UPLINK</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>10.32.</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>loopback</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>10.32.20.254</t>
   </si>
   <si>
     <t>255.255.255.0</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>1.1.1.1</t>
   </si>
   <si>
@@ -65,6 +92,9 @@
   </si>
   <si>
     <t>typo</t>
+  </si>
+  <si>
+    <t>45</t>
   </si>
 </sst>
 </file>
@@ -101,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -111,6 +141,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -168,126 +199,151 @@
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>254.0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>254.0</v>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>16.0</v>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>17.0</v>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>18.0</v>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>19.0</v>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1.0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5.0</v>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2">
-        <v>45.0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.0</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>